<commit_message>
Linked to GPIOLayout.py & chose pin for DuckShoot.
</commit_message>
<xml_diff>
--- a/Design/Chassis Design/GPIO Pins.xlsx
+++ b/Design/Chassis Design/GPIO Pins.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="698" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="698" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Current GPIO Pins - Robohat" sheetId="1" r:id="rId1"/>
     <sheet name="GPIO Pins - L298N" sheetId="2" r:id="rId2"/>
+    <sheet name="GPIO Pins - L298N 33.3.18" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>Pin No.</t>
   </si>
@@ -57,13 +58,67 @@
   </si>
   <si>
     <t>Right Motor - Rear</t>
+  </si>
+  <si>
+    <t>MOTOR_LEFT_FRONT_FORWARD_PIN</t>
+  </si>
+  <si>
+    <t>MOTOR_LEFT_FRONT_BACKWARD_PIN</t>
+  </si>
+  <si>
+    <t>MOTOR_LEFT_REAR_FORWARD_PIN</t>
+  </si>
+  <si>
+    <t>MOTOR_LEFT_REAR_BACKWARD_PIN</t>
+  </si>
+  <si>
+    <t>MOTOR_RIGHT_FRONT_FORWARD_PIN</t>
+  </si>
+  <si>
+    <t>MOTOR_RIGHT_FRONT_BACKWARD_PIN</t>
+  </si>
+  <si>
+    <t>MOTOR_RIGHT_REAR_FORWARD_PIN</t>
+  </si>
+  <si>
+    <t>MOTOR_RIGHT_REAR_BACKWARD_PIN</t>
+  </si>
+  <si>
+    <t>SONAR_FRONT_RX_PIN</t>
+  </si>
+  <si>
+    <t>SONAR_FRONT_TX_PIN / SONAR_FRONT_RX_PIN</t>
+  </si>
+  <si>
+    <t>SONAR_LEFT_TX_PIN</t>
+  </si>
+  <si>
+    <t>SONAR_LEFT_RX_PIN</t>
+  </si>
+  <si>
+    <t>SONAR_RIGHT_TX_PIN</t>
+  </si>
+  <si>
+    <t>SONAR_RIGHT_RX_PIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVO_VERTICAL_PIN </t>
+  </si>
+  <si>
+    <t>SERVO_HORIZONTAL_PIN</t>
+  </si>
+  <si>
+    <t>DUCK_SHOOT_FIRE</t>
+  </si>
+  <si>
+    <t>GPIO Pin No. Mapped to GPIOLayout.py</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,8 +134,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +167,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -127,12 +228,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -144,6 +242,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -261,6 +381,66 @@
         <a:xfrm>
           <a:off x="3617855" y="114300"/>
           <a:ext cx="6278618" cy="4705350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>10166</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2028822</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Image result for gpio raspberry pi"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="409574" y="4582166"/>
+          <a:ext cx="5248273" cy="3933184"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -584,65 +764,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>7</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2">
         <v>9</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>11</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -650,24 +830,24 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>13</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>15</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -675,11 +855,11 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2">
         <v>17</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -687,20 +867,20 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2">
         <v>19</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2">
         <v>21</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -708,51 +888,51 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2">
         <v>23</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2">
         <v>25</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2">
         <v>27</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>29</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>31</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -760,24 +940,24 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>33</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>35</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -785,13 +965,13 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>37</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>38</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -799,14 +979,14 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="2">
         <v>39</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>40</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -824,7 +1004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -837,65 +1017,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2">
         <v>5</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>7</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2">
         <v>9</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>11</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -903,24 +1083,24 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>13</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>15</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -928,11 +1108,11 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="2">
         <v>17</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>18</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -940,20 +1120,20 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="2">
         <v>19</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="2">
         <v>21</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -961,51 +1141,51 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="2">
         <v>23</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="2">
         <v>25</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="2">
         <v>27</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>29</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="3">
         <v>31</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>32</v>
       </c>
       <c r="D18" s="1" t="s">
@@ -1013,24 +1193,24 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B19" s="3">
         <v>33</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B20" s="3">
         <v>35</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -1038,13 +1218,13 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B21" s="3">
         <v>37</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <v>38</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -1052,15 +1232,273 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="2">
         <v>39</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <v>40</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="45.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="12">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="12">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3">
+        <v>7</v>
+      </c>
+      <c r="C6" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="9">
+        <v>9</v>
+      </c>
+      <c r="C7" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3">
+        <v>13</v>
+      </c>
+      <c r="C9" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="8">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="10">
+        <v>19</v>
+      </c>
+      <c r="C12" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="10">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="10">
+        <v>23</v>
+      </c>
+      <c r="C14" s="10">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="9">
+        <v>25</v>
+      </c>
+      <c r="C15" s="10">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="13">
+        <v>27</v>
+      </c>
+      <c r="C16" s="13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="3">
+        <v>29</v>
+      </c>
+      <c r="C17" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="3">
+        <v>31</v>
+      </c>
+      <c r="C18" s="3">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3">
+        <v>33</v>
+      </c>
+      <c r="C19" s="9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3">
+        <v>36</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="3">
+        <v>37</v>
+      </c>
+      <c r="C21" s="3">
+        <v>38</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="9">
+        <v>39</v>
+      </c>
+      <c r="C22" s="3">
+        <v>40</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>